<commit_message>
Update CAM 532-LMO Li content
</commit_message>
<xml_diff>
--- a/example notebooks/Example publication - integrated modelling/data/ODYM_database/3_MC_element_goods_v2.xlsx
+++ b/example notebooks/Example publication - integrated modelling/data/ODYM_database/3_MC_element_goods_v2.xlsx
@@ -15,7 +15,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Values_Master!$A$1:$E$71</definedName>
   </definedNames>
-  <calcPr calcId="191029" iterate="1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -545,8 +545,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="&quot; &quot;#,##0.00&quot; &quot;;&quot;-&quot;#,##0.00&quot; &quot;;&quot; -&quot;00&quot; &quot;;&quot; &quot;@&quot; &quot;"/>
-    <numFmt numFmtId="170" formatCode="0.000000"/>
+    <numFmt numFmtId="164" formatCode="&quot; &quot;#,##0.00&quot; &quot;;&quot;-&quot;#,##0.00&quot; &quot;;&quot; -&quot;00&quot; &quot;;&quot; &quot;@&quot; &quot;"/>
+    <numFmt numFmtId="165" formatCode="0.000000"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -1071,7 +1071,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
@@ -1120,7 +1120,7 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1192,6 +1192,8 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1201,8 +1203,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="15">
     <cellStyle name="Body: normal cell" xfId="5" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -2025,8 +2025,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0478C09-3B6A-4E3E-8C6B-6D4AB899ADBA}">
   <dimension ref="A1:E71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3171,7 +3171,7 @@
   <dimension ref="A2:R33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3202,7 +3202,7 @@
       <c r="O2" s="2"/>
     </row>
     <row r="3" spans="1:15" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A3" s="67" t="s">
+      <c r="A3" s="64" t="s">
         <v>155</v>
       </c>
       <c r="C3" s="22"/>
@@ -3254,47 +3254,47 @@
         <v>76</v>
       </c>
       <c r="B6" s="29">
-        <f ca="1">OFFSET($F$21,  MATCH($A6, $A$22:$A$31,0), MATCH(B$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(B$5, $G$20:$Q$20, 0)) /$B22</f>
+        <f t="shared" ref="B6:B14" ca="1" si="0">OFFSET($F$21,  MATCH($A6, $A$22:$A$31,0), MATCH(B$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(B$5, $G$20:$Q$20, 0)) /$B22</f>
         <v>7.1984876122741057E-2</v>
       </c>
       <c r="C6" s="29">
-        <f t="shared" ref="C6:L6" ca="1" si="0">OFFSET($F$21,  MATCH($A6, $A$22:$A$31,0), MATCH(C$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(C$5, $G$20:$Q$20, 0)) /$B22</f>
+        <f t="shared" ref="C6:L6" ca="1" si="1">OFFSET($F$21,  MATCH($A6, $A$22:$A$31,0), MATCH(C$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(C$5, $G$20:$Q$20, 0)) /$B22</f>
         <v>0.20278606364500296</v>
       </c>
       <c r="D6" s="29">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0.18976437296297841</v>
       </c>
       <c r="E6" s="29">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0.20354595010390092</v>
       </c>
       <c r="F6" s="29">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="G6" s="29">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="H6" s="29">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="I6" s="29">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="J6" s="29">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0.33191873716537662</v>
       </c>
       <c r="K6" s="29">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="L6" s="29">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -3303,47 +3303,47 @@
         <v>77</v>
       </c>
       <c r="B7" s="29">
-        <f ca="1">OFFSET($F$21,  MATCH($A7, $A$22:$A$31,0), MATCH(B$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(B$5, $G$20:$Q$20, 0)) /$B23</f>
+        <f t="shared" ca="1" si="0"/>
         <v>7.1590674644109759E-2</v>
       </c>
       <c r="C7" s="29">
-        <f ca="1">OFFSET($F$21,  MATCH($A7, $A$22:$A$31,0), MATCH(C$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(C$5, $G$20:$Q$20, 0)) /$B23</f>
+        <f t="shared" ref="C7:L7" ca="1" si="2">OFFSET($F$21,  MATCH($A7, $A$22:$A$31,0), MATCH(C$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(C$5, $G$20:$Q$20, 0)) /$B23</f>
         <v>0.36337940994429546</v>
       </c>
       <c r="D7" s="29">
-        <f ca="1">OFFSET($F$21,  MATCH($A7, $A$22:$A$31,0), MATCH(D$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(D$5, $G$20:$Q$20, 0)) /$B23</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0.11334846296678358</v>
       </c>
       <c r="E7" s="29">
-        <f ca="1">OFFSET($F$21,  MATCH($A7, $A$22:$A$31,0), MATCH(E$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(E$5, $G$20:$Q$20, 0)) /$B23</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0.12158035898493916</v>
       </c>
       <c r="F7" s="29">
-        <f ca="1">OFFSET($F$21,  MATCH($A7, $A$22:$A$31,0), MATCH(F$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(F$5, $G$20:$Q$20, 0)) /$B23</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="G7" s="29">
-        <f ca="1">OFFSET($F$21,  MATCH($A7, $A$22:$A$31,0), MATCH(G$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(G$5, $G$20:$Q$20, 0)) /$B23</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="H7" s="29">
-        <f ca="1">OFFSET($F$21,  MATCH($A7, $A$22:$A$31,0), MATCH(H$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(H$5, $G$20:$Q$20, 0)) /$B23</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="I7" s="29">
-        <f ca="1">OFFSET($F$21,  MATCH($A7, $A$22:$A$31,0), MATCH(I$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(I$5, $G$20:$Q$20, 0)) /$B23</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="J7" s="29">
-        <f ca="1">OFFSET($F$21,  MATCH($A7, $A$22:$A$31,0), MATCH(J$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(J$5, $G$20:$Q$20, 0)) /$B23</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0.3301010934598721</v>
       </c>
       <c r="K7" s="29">
-        <f ca="1">OFFSET($F$21,  MATCH($A7, $A$22:$A$31,0), MATCH(K$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(K$5, $G$20:$Q$20, 0)) /$B23</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="L7" s="29">
-        <f ca="1">OFFSET($F$21,  MATCH($A7, $A$22:$A$31,0), MATCH(L$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(L$5, $G$20:$Q$20, 0)) /$B23</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -3352,47 +3352,47 @@
         <v>78</v>
       </c>
       <c r="B8" s="29">
-        <f ca="1">OFFSET($F$21,  MATCH($A8, $A$22:$A$31,0), MATCH(B$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(B$5, $G$20:$Q$20, 0)) /$B24</f>
+        <f t="shared" ca="1" si="0"/>
         <v>7.1870178018495698E-2</v>
       </c>
       <c r="C8" s="29">
-        <f ca="1">OFFSET($F$21,  MATCH($A8, $A$22:$A$31,0), MATCH(C$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(C$5, $G$20:$Q$20, 0)) /$B24</f>
+        <f t="shared" ref="C8:L8" ca="1" si="3">OFFSET($F$21,  MATCH($A8, $A$22:$A$31,0), MATCH(C$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(C$5, $G$20:$Q$20, 0)) /$B24</f>
         <v>0.30399842589811832</v>
       </c>
       <c r="D8" s="29">
-        <f ca="1">OFFSET($F$21,  MATCH($A8, $A$22:$A$31,0), MATCH(D$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(D$5, $G$20:$Q$20, 0)) /$B24</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0.17068649482721124</v>
       </c>
       <c r="E8" s="29">
-        <f ca="1">OFFSET($F$21,  MATCH($A8, $A$22:$A$31,0), MATCH(E$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(E$5, $G$20:$Q$20, 0)) /$B24</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0.12205503143025798</v>
       </c>
       <c r="F8" s="29">
-        <f ca="1">OFFSET($F$21,  MATCH($A8, $A$22:$A$31,0), MATCH(F$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(F$5, $G$20:$Q$20, 0)) /$B24</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="G8" s="29">
-        <f ca="1">OFFSET($F$21,  MATCH($A8, $A$22:$A$31,0), MATCH(G$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(G$5, $G$20:$Q$20, 0)) /$B24</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="H8" s="29">
-        <f ca="1">OFFSET($F$21,  MATCH($A8, $A$22:$A$31,0), MATCH(H$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(H$5, $G$20:$Q$20, 0)) /$B24</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="I8" s="29">
-        <f ca="1">OFFSET($F$21,  MATCH($A8, $A$22:$A$31,0), MATCH(I$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(I$5, $G$20:$Q$20, 0)) /$B24</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="J8" s="29">
-        <f ca="1">OFFSET($F$21,  MATCH($A8, $A$22:$A$31,0), MATCH(J$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(J$5, $G$20:$Q$20, 0)) /$B24</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0.33138986982591673</v>
       </c>
       <c r="K8" s="29">
-        <f ca="1">OFFSET($F$21,  MATCH($A8, $A$22:$A$31,0), MATCH(K$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(K$5, $G$20:$Q$20, 0)) /$B24</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="L8" s="29">
-        <f ca="1">OFFSET($F$21,  MATCH($A8, $A$22:$A$31,0), MATCH(L$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(L$5, $G$20:$Q$20, 0)) /$B24</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -3401,47 +3401,47 @@
         <v>79</v>
       </c>
       <c r="B9" s="29">
-        <f ca="1">OFFSET($F$21,  MATCH($A9, $A$22:$A$31,0), MATCH(B$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(B$5, $G$20:$Q$20, 0)) /$B25</f>
+        <f t="shared" ca="1" si="0"/>
         <v>7.132946194562928E-2</v>
       </c>
       <c r="C9" s="29">
-        <f ca="1">OFFSET($F$21,  MATCH($A9, $A$22:$A$31,0), MATCH(C$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(C$5, $G$20:$Q$20, 0)) /$B25</f>
+        <f t="shared" ref="C9:L9" ca="1" si="4">OFFSET($F$21,  MATCH($A9, $A$22:$A$31,0), MATCH(C$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(C$5, $G$20:$Q$20, 0)) /$B25</f>
         <v>0.48273806464874869</v>
       </c>
       <c r="D9" s="29">
-        <f ca="1">OFFSET($F$21,  MATCH($A9, $A$22:$A$31,0), MATCH(D$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(D$5, $G$20:$Q$20, 0)) /$B25</f>
+        <f t="shared" ca="1" si="4"/>
         <v>5.6467444370214295E-2</v>
       </c>
       <c r="E9" s="29">
-        <f ca="1">OFFSET($F$21,  MATCH($A9, $A$22:$A$31,0), MATCH(E$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(E$5, $G$20:$Q$20, 0)) /$B25</f>
+        <f t="shared" ca="1" si="4"/>
         <v>6.0568374531065325E-2</v>
       </c>
       <c r="F9" s="29">
-        <f ca="1">OFFSET($F$21,  MATCH($A9, $A$22:$A$31,0), MATCH(F$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(F$5, $G$20:$Q$20, 0)) /$B25</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
       <c r="G9" s="29">
-        <f ca="1">OFFSET($F$21,  MATCH($A9, $A$22:$A$31,0), MATCH(G$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(G$5, $G$20:$Q$20, 0)) /$B25</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
       <c r="H9" s="29">
-        <f ca="1">OFFSET($F$21,  MATCH($A9, $A$22:$A$31,0), MATCH(H$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(H$5, $G$20:$Q$20, 0)) /$B25</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
       <c r="I9" s="29">
-        <f ca="1">OFFSET($F$21,  MATCH($A9, $A$22:$A$31,0), MATCH(I$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(I$5, $G$20:$Q$20, 0)) /$B25</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
       <c r="J9" s="29">
-        <f ca="1">OFFSET($F$21,  MATCH($A9, $A$22:$A$31,0), MATCH(J$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(J$5, $G$20:$Q$20, 0)) /$B25</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0.32889665450434247</v>
       </c>
       <c r="K9" s="29">
-        <f ca="1">OFFSET($F$21,  MATCH($A9, $A$22:$A$31,0), MATCH(K$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(K$5, $G$20:$Q$20, 0)) /$B25</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
       <c r="L9" s="29">
-        <f ca="1">OFFSET($F$21,  MATCH($A9, $A$22:$A$31,0), MATCH(L$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(L$5, $G$20:$Q$20, 0)) /$B25</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -3450,47 +3450,47 @@
         <v>80</v>
       </c>
       <c r="B10" s="29">
-        <f ca="1">OFFSET($F$21,  MATCH($A10, $A$22:$A$31,0), MATCH(B$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(B$5, $G$20:$Q$20, 0)) /$B26</f>
+        <f t="shared" ca="1" si="0"/>
         <v>7.22190714542153E-2</v>
       </c>
       <c r="C10" s="29">
-        <f ca="1">OFFSET($F$21,  MATCH($A10, $A$22:$A$31,0), MATCH(C$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(C$5, $G$20:$Q$20, 0)) /$B26</f>
+        <f t="shared" ref="C10:L10" ca="1" si="5">OFFSET($F$21,  MATCH($A10, $A$22:$A$31,0), MATCH(C$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(C$5, $G$20:$Q$20, 0)) /$B26</f>
         <v>0.48875869568610719</v>
       </c>
       <c r="D10" s="29">
-        <f ca="1">OFFSET($F$21,  MATCH($A10, $A$22:$A$31,0), MATCH(D$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(D$5, $G$20:$Q$20, 0)) /$B26</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
       <c r="E10" s="29">
-        <f ca="1">OFFSET($F$21,  MATCH($A10, $A$22:$A$31,0), MATCH(E$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(E$5, $G$20:$Q$20, 0)) /$B26</f>
+        <f t="shared" ca="1" si="5"/>
         <v>9.1985660247771758E-2</v>
       </c>
       <c r="F10" s="29">
-        <f ca="1">OFFSET($F$21,  MATCH($A10, $A$22:$A$31,0), MATCH(F$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(F$5, $G$20:$Q$20, 0)) /$B26</f>
+        <f t="shared" ca="1" si="5"/>
         <v>1.4037972246647903E-2</v>
       </c>
       <c r="G10" s="29">
-        <f ca="1">OFFSET($F$21,  MATCH($A10, $A$22:$A$31,0), MATCH(G$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(G$5, $G$20:$Q$20, 0)) /$B26</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
       <c r="H10" s="29">
-        <f ca="1">OFFSET($F$21,  MATCH($A10, $A$22:$A$31,0), MATCH(H$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(H$5, $G$20:$Q$20, 0)) /$B26</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
       <c r="I10" s="29">
-        <f ca="1">OFFSET($F$21,  MATCH($A10, $A$22:$A$31,0), MATCH(I$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(I$5, $G$20:$Q$20, 0)) /$B26</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
       <c r="J10" s="29">
-        <f ca="1">OFFSET($F$21,  MATCH($A10, $A$22:$A$31,0), MATCH(J$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(J$5, $G$20:$Q$20, 0)) /$B26</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0.3329986003652578</v>
       </c>
       <c r="K10" s="29">
-        <f ca="1">OFFSET($F$21,  MATCH($A10, $A$22:$A$31,0), MATCH(K$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(K$5, $G$20:$Q$20, 0)) /$B26</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
       <c r="L10" s="29">
-        <f ca="1">OFFSET($F$21,  MATCH($A10, $A$22:$A$31,0), MATCH(L$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(L$5, $G$20:$Q$20, 0)) /$B26</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -3499,47 +3499,47 @@
         <v>66</v>
       </c>
       <c r="B11" s="29">
-        <f ca="1">OFFSET($F$21,  MATCH($A11, $A$22:$A$31,0), MATCH(B$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(B$5, $G$20:$Q$20, 0)) /$B27</f>
+        <f t="shared" ca="1" si="0"/>
         <v>4.3990872210953352E-2</v>
       </c>
       <c r="C11" s="29">
-        <f ca="1">OFFSET($F$21,  MATCH($A11, $A$22:$A$31,0), MATCH(C$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(C$5, $G$20:$Q$20, 0)) /$B27</f>
+        <f t="shared" ref="C11:L11" ca="1" si="6">OFFSET($F$21,  MATCH($A11, $A$22:$A$31,0), MATCH(C$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(C$5, $G$20:$Q$20, 0)) /$B27</f>
         <v>0</v>
       </c>
       <c r="D11" s="29">
-        <f ca="1">OFFSET($F$21,  MATCH($A11, $A$22:$A$31,0), MATCH(D$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(D$5, $G$20:$Q$20, 0)) /$B27</f>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
       <c r="E11" s="29">
-        <f ca="1">OFFSET($F$21,  MATCH($A11, $A$22:$A$31,0), MATCH(E$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(E$5, $G$20:$Q$20, 0)) /$B27</f>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
       <c r="F11" s="29">
-        <f ca="1">OFFSET($F$21,  MATCH($A11, $A$22:$A$31,0), MATCH(F$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(F$5, $G$20:$Q$20, 0)) /$B27</f>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
       <c r="G11" s="29">
-        <f ca="1">OFFSET($F$21,  MATCH($A11, $A$22:$A$31,0), MATCH(G$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(G$5, $G$20:$Q$20, 0)) /$B27</f>
+        <f t="shared" ca="1" si="6"/>
         <v>0.35401876267748483</v>
       </c>
       <c r="H11" s="29">
-        <f ca="1">OFFSET($F$21,  MATCH($A11, $A$22:$A$31,0), MATCH(H$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(H$5, $G$20:$Q$20, 0)) /$B27</f>
+        <f t="shared" ca="1" si="6"/>
         <v>0.1963108519269777</v>
       </c>
       <c r="I11" s="29">
-        <f ca="1">OFFSET($F$21,  MATCH($A11, $A$22:$A$31,0), MATCH(I$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(I$5, $G$20:$Q$20, 0)) /$B27</f>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
       <c r="J11" s="29">
-        <f ca="1">OFFSET($F$21,  MATCH($A11, $A$22:$A$31,0), MATCH(J$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(J$5, $G$20:$Q$20, 0)) /$B27</f>
+        <f t="shared" ca="1" si="6"/>
         <v>0.40567951318458423</v>
       </c>
       <c r="K11" s="29">
-        <f ca="1">OFFSET($F$21,  MATCH($A11, $A$22:$A$31,0), MATCH(K$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(K$5, $G$20:$Q$20, 0)) /$B27</f>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
       <c r="L11" s="29">
-        <f ca="1">OFFSET($F$21,  MATCH($A11, $A$22:$A$31,0), MATCH(L$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(L$5, $G$20:$Q$20, 0)) /$B27</f>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -3548,47 +3548,47 @@
         <v>83</v>
       </c>
       <c r="B12" s="29">
-        <f ca="1">OFFSET($F$21,  MATCH($A12, $A$22:$A$31,0), MATCH(B$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(B$5, $G$20:$Q$20, 0)) /$B28</f>
+        <f t="shared" ca="1" si="0"/>
         <v>4.3370071582774693E-2</v>
       </c>
       <c r="C12" s="29">
-        <f ca="1">OFFSET($F$21,  MATCH($A12, $A$22:$A$31,0), MATCH(C$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(C$5, $G$20:$Q$20, 0)) /$B28</f>
+        <f t="shared" ref="C12:L12" ca="1" si="7">OFFSET($F$21,  MATCH($A12, $A$22:$A$31,0), MATCH(C$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(C$5, $G$20:$Q$20, 0)) /$B28</f>
         <v>0</v>
       </c>
       <c r="D12" s="29">
-        <f ca="1">OFFSET($F$21,  MATCH($A12, $A$22:$A$31,0), MATCH(D$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(D$5, $G$20:$Q$20, 0)) /$B28</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0.59303488239972735</v>
       </c>
       <c r="E12" s="29">
-        <f ca="1">OFFSET($F$21,  MATCH($A12, $A$22:$A$31,0), MATCH(E$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(E$5, $G$20:$Q$20, 0)) /$B28</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
       <c r="F12" s="29">
-        <f ca="1">OFFSET($F$21,  MATCH($A12, $A$22:$A$31,0), MATCH(F$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(F$5, $G$20:$Q$20, 0)) /$B28</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
       <c r="G12" s="29">
-        <f ca="1">OFFSET($F$21,  MATCH($A12, $A$22:$A$31,0), MATCH(G$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(G$5, $G$20:$Q$20, 0)) /$B28</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
       <c r="H12" s="29">
-        <f ca="1">OFFSET($F$21,  MATCH($A12, $A$22:$A$31,0), MATCH(H$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(H$5, $G$20:$Q$20, 0)) /$B28</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
       <c r="I12" s="29">
-        <f ca="1">OFFSET($F$21,  MATCH($A12, $A$22:$A$31,0), MATCH(I$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(I$5, $G$20:$Q$20, 0)) /$B28</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
       <c r="J12" s="29">
-        <f ca="1">OFFSET($F$21,  MATCH($A12, $A$22:$A$31,0), MATCH(J$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(J$5, $G$20:$Q$20, 0)) /$B28</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0.36359504601749804</v>
       </c>
       <c r="K12" s="29">
-        <f ca="1">OFFSET($F$21,  MATCH($A12, $A$22:$A$31,0), MATCH(K$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(K$5, $G$20:$Q$20, 0)) /$B28</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
       <c r="L12" s="29">
-        <f ca="1">OFFSET($F$21,  MATCH($A12, $A$22:$A$31,0), MATCH(L$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(L$5, $G$20:$Q$20, 0)) /$B28</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -3597,47 +3597,47 @@
         <v>85</v>
       </c>
       <c r="B13" s="29">
-        <f ca="1">OFFSET($F$21,  MATCH($A13, $A$22:$A$31,0), MATCH(B$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(B$5, $G$20:$Q$20, 0)) /$B29</f>
+        <f t="shared" ca="1" si="0"/>
         <v>6.0445063798284203E-2</v>
       </c>
       <c r="C13" s="29">
-        <f ca="1">OFFSET($F$21,  MATCH($A13, $A$22:$A$31,0), MATCH(C$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(C$5, $G$20:$Q$20, 0)) /$B29</f>
+        <f t="shared" ref="C13:L13" ca="1" si="8">OFFSET($F$21,  MATCH($A13, $A$22:$A$31,0), MATCH(C$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(C$5, $G$20:$Q$20, 0)) /$B29</f>
         <v>0</v>
       </c>
       <c r="D13" s="29">
-        <f ca="1">OFFSET($F$21,  MATCH($A13, $A$22:$A$31,0), MATCH(D$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(D$5, $G$20:$Q$20, 0)) /$B29</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
       <c r="E13" s="29">
-        <f ca="1">OFFSET($F$21,  MATCH($A13, $A$22:$A$31,0), MATCH(E$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(E$5, $G$20:$Q$20, 0)) /$B29</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
       <c r="F13" s="29">
-        <f ca="1">OFFSET($F$21,  MATCH($A13, $A$22:$A$31,0), MATCH(F$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(F$5, $G$20:$Q$20, 0)) /$B29</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
       <c r="G13" s="29">
-        <f ca="1">OFFSET($F$21,  MATCH($A13, $A$22:$A$31,0), MATCH(G$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(G$5, $G$20:$Q$20, 0)) /$B29</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
       <c r="H13" s="29">
-        <f ca="1">OFFSET($F$21,  MATCH($A13, $A$22:$A$31,0), MATCH(H$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(H$5, $G$20:$Q$20, 0)) /$B29</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
       <c r="I13" s="29">
-        <f ca="1">OFFSET($F$21,  MATCH($A13, $A$22:$A$31,0), MATCH(I$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(I$5, $G$20:$Q$20, 0)) /$B29</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0.5214910943692026</v>
       </c>
       <c r="J13" s="29">
-        <f ca="1">OFFSET($F$21,  MATCH($A13, $A$22:$A$31,0), MATCH(J$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(J$5, $G$20:$Q$20, 0)) /$B29</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0.41806384183251316</v>
       </c>
       <c r="K13" s="29">
-        <f ca="1">OFFSET($F$21,  MATCH($A13, $A$22:$A$31,0), MATCH(K$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(K$5, $G$20:$Q$20, 0)) /$B29</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
       <c r="L13" s="29">
-        <f ca="1">OFFSET($F$21,  MATCH($A13, $A$22:$A$31,0), MATCH(L$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(L$5, $G$20:$Q$20, 0)) /$B29</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -3646,47 +3646,47 @@
         <v>87</v>
       </c>
       <c r="B14" s="29">
-        <f ca="1">OFFSET($F$21,  MATCH($A14, $A$22:$A$31,0), MATCH(B$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(B$5, $G$20:$Q$20, 0)) /$B30</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
       <c r="C14" s="29">
-        <f ca="1">OFFSET($F$21,  MATCH($A14, $A$22:$A$31,0), MATCH(C$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(C$5, $G$20:$Q$20, 0)) /$B30</f>
+        <f t="shared" ref="C14:L14" ca="1" si="9">OFFSET($F$21,  MATCH($A14, $A$22:$A$31,0), MATCH(C$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(C$5, $G$20:$Q$20, 0)) /$B30</f>
         <v>0</v>
       </c>
       <c r="D14" s="29">
-        <f ca="1">OFFSET($F$21,  MATCH($A14, $A$22:$A$31,0), MATCH(D$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(D$5, $G$20:$Q$20, 0)) /$B30</f>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
       <c r="E14" s="29">
-        <f ca="1">OFFSET($F$21,  MATCH($A14, $A$22:$A$31,0), MATCH(E$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(E$5, $G$20:$Q$20, 0)) /$B30</f>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
       <c r="F14" s="29">
-        <f ca="1">OFFSET($F$21,  MATCH($A14, $A$22:$A$31,0), MATCH(F$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(F$5, $G$20:$Q$20, 0)) /$B30</f>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
       <c r="G14" s="29">
-        <f ca="1">OFFSET($F$21,  MATCH($A14, $A$22:$A$31,0), MATCH(G$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(G$5, $G$20:$Q$20, 0)) /$B30</f>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
       <c r="H14" s="29">
-        <f ca="1">OFFSET($F$21,  MATCH($A14, $A$22:$A$31,0), MATCH(H$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(H$5, $G$20:$Q$20, 0)) /$B30</f>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
       <c r="I14" s="29">
-        <f ca="1">OFFSET($F$21,  MATCH($A14, $A$22:$A$31,0), MATCH(I$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(I$5, $G$20:$Q$20, 0)) /$B30</f>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
       <c r="J14" s="29">
-        <f ca="1">OFFSET($F$21,  MATCH($A14, $A$22:$A$31,0), MATCH(J$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(J$5, $G$20:$Q$20, 0)) /$B30</f>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
       <c r="K14" s="29">
-        <f ca="1">OFFSET($F$21,  MATCH($A14, $A$22:$A$31,0), MATCH(K$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(K$5, $G$20:$Q$20, 0)) /$B30</f>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
       <c r="L14" s="29">
-        <f ca="1">OFFSET($F$21,  MATCH($A14, $A$22:$A$31,0), MATCH(L$5, $G$20:$Q$20, 0))*INDEX($G$21:$Q$21, MATCH(L$5, $G$20:$Q$20, 0)) /$B30</f>
+        <f t="shared" ca="1" si="9"/>
         <v>1</v>
       </c>
     </row>
@@ -3713,58 +3713,58 @@
         <v>5.7620124800635192E-2</v>
       </c>
       <c r="C16" s="29">
-        <f t="shared" ref="C16:L16" ca="1" si="1">(C8*0.5)+(C12*0.5)</f>
+        <f t="shared" ref="C16:L16" ca="1" si="10">(C8*0.5)+(C12*0.5)</f>
         <v>0.15199921294905916</v>
       </c>
       <c r="D16" s="29">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="10"/>
         <v>0.38186068861346928</v>
       </c>
       <c r="E16" s="29">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="10"/>
         <v>6.1027515715128988E-2</v>
       </c>
       <c r="F16" s="29">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
       <c r="G16" s="29">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
       <c r="H16" s="29">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
       <c r="I16" s="29">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
       <c r="J16" s="29">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="10"/>
         <v>0.34749245792170735</v>
       </c>
       <c r="K16" s="29">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
       <c r="L16" s="29">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="66" t="s">
+      <c r="A18" s="63" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="19" spans="1:18" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="63" t="s">
+      <c r="A19" s="65" t="s">
         <v>143</v>
       </c>
-      <c r="B19" s="64"/>
-      <c r="C19" s="64"/>
-      <c r="D19" s="65"/>
+      <c r="B19" s="66"/>
+      <c r="C19" s="66"/>
+      <c r="D19" s="67"/>
       <c r="E19" s="30"/>
       <c r="F19" s="31"/>
       <c r="G19" s="32"/>
@@ -3933,7 +3933,7 @@
         <v>180</v>
       </c>
       <c r="D23" s="44">
-        <f t="shared" ref="D23:D29" si="2">G23/3600*1000*96485/B23</f>
+        <f t="shared" ref="D23:D29" si="11">G23/3600*1000*96485/B23</f>
         <v>276.47399307704654</v>
       </c>
       <c r="E23" s="44" t="s">
@@ -3978,7 +3978,7 @@
         <v>161</v>
       </c>
       <c r="D24" s="44">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>277.55339922008318</v>
       </c>
       <c r="E24" s="44" t="s">
@@ -4023,7 +4023,7 @@
         <v>212</v>
       </c>
       <c r="D25" s="44">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>275.46522317579411</v>
       </c>
       <c r="E25" s="44" t="s">
@@ -4068,7 +4068,7 @@
         <v>200</v>
       </c>
       <c r="D26" s="44">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>278.90078087015542</v>
       </c>
       <c r="E26" s="44" t="s">
@@ -4110,7 +4110,7 @@
         <v>150</v>
       </c>
       <c r="D27" s="44">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>169.88709995492451</v>
       </c>
       <c r="E27" s="44" t="s">
@@ -4150,7 +4150,7 @@
         <v>108</v>
       </c>
       <c r="D28" s="44">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>167.48964764105094</v>
       </c>
       <c r="E28" s="44" t="s">
@@ -4188,7 +4188,7 @@
         <v>170</v>
       </c>
       <c r="D29" s="44">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>233.43107511116921</v>
       </c>
       <c r="E29" s="44" t="s">

</xml_diff>